<commit_message>
Changes to Base code + Cluster with new features.
Changes to Base code + Cluster with new features.
</commit_message>
<xml_diff>
--- a/documentation/week2/Feature_selection.xlsx
+++ b/documentation/week2/Feature_selection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharakumarrathinar/Documents/MS_Heriot_Watt/Course_work/F21DL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharakumarrathinar/Documents/MS_Heriot_Watt/Course_work/F21DL/code/documentation/week2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3966F1-34E2-E34A-AED7-1FDAC6A753AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A2A5C9-A8F5-E543-9406-479339A3E85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20960" xr2:uid="{416BFC02-E214-EC46-9E71-DF9EF0F7F4BC}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20960" activeTab="3" xr2:uid="{416BFC02-E214-EC46-9E71-DF9EF0F7F4BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Feature Score" sheetId="3" r:id="rId3"/>
     <sheet name="Detail Score Calc" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -393,6 +393,18 @@
   </si>
   <si>
     <t>Total Delay</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Lasso</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>RFE</t>
   </si>
 </sst>
 </file>
@@ -500,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -508,16 +520,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -855,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F66A96FF-C1D7-DC48-90A1-A2229DAD05FB}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+    <sheetView zoomScale="108" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -2006,30 +2017,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="I1" s="8" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="O1" s="8" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="O1" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="5" t="s">
@@ -2085,7 +2096,7 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -2094,13 +2105,13 @@
       <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="5">
@@ -2119,7 +2130,7 @@
         <f>AVERAGE(J3,K3,L3)</f>
         <v>7</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="5">
@@ -2143,7 +2154,7 @@
       <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -2152,13 +2163,13 @@
       <c r="E4" s="5">
         <v>2</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="5">
@@ -2177,7 +2188,7 @@
         <f t="shared" ref="N4:N22" si="0">AVERAGE(J4,K4,L4)</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="O4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="P4" s="5">
@@ -2193,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:T23" si="1">AVERAGE(P4,Q4,R4)</f>
+        <f t="shared" ref="T4:T14" si="1">AVERAGE(P4,Q4,R4)</f>
         <v>2.3333333333333335</v>
       </c>
     </row>
@@ -2201,7 +2212,7 @@
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -2210,13 +2221,13 @@
       <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="7" t="s">
         <v>25</v>
       </c>
       <c r="J5" s="5">
@@ -2235,7 +2246,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="P5" s="5">
@@ -2259,7 +2270,7 @@
       <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -2268,13 +2279,13 @@
       <c r="E6" s="5">
         <v>4</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="5">
@@ -2293,7 +2304,7 @@
         <f t="shared" si="0"/>
         <v>4.666666666666667</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="P6" s="5">
@@ -2317,7 +2328,7 @@
       <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -2326,13 +2337,13 @@
       <c r="E7" s="5">
         <v>5</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="J7" s="5">
@@ -2351,7 +2362,7 @@
         <f t="shared" si="0"/>
         <v>6.333333333333333</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="7" t="s">
         <v>25</v>
       </c>
       <c r="P7" s="5">
@@ -2375,7 +2386,7 @@
       <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -2384,13 +2395,13 @@
       <c r="E8" s="5">
         <v>6</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="5">
@@ -2409,7 +2420,7 @@
         <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="O8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="P8" s="5">
@@ -2433,7 +2444,7 @@
       <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -2442,13 +2453,13 @@
       <c r="E9" s="5">
         <v>7</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>18</v>
       </c>
       <c r="J9" s="5">
@@ -2467,7 +2478,7 @@
         <f>AVERAGE(J9,K9,L9)</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="P9" s="5">
@@ -2491,7 +2502,7 @@
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -2500,13 +2511,13 @@
       <c r="E10" s="5">
         <v>8</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J10" s="5">
@@ -2525,7 +2536,7 @@
         <f>AVERAGE(J10,K10,L10)</f>
         <v>9</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="O10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="P10" s="5">
@@ -2549,7 +2560,7 @@
       <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -2558,13 +2569,13 @@
       <c r="E11" s="5">
         <v>9</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J11" s="5">
@@ -2583,7 +2594,7 @@
         <f t="shared" si="0"/>
         <v>9.6666666666666661</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="P11" s="5">
@@ -2607,7 +2618,7 @@
       <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -2616,13 +2627,13 @@
       <c r="E12" s="5">
         <v>10</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="J12" s="5">
@@ -2641,7 +2652,7 @@
         <f>AVERAGE(J12,K12,L12)</f>
         <v>9.6666666666666661</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="O12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="P12" s="5">
@@ -2665,7 +2676,7 @@
       <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -2674,13 +2685,13 @@
       <c r="E13" s="5">
         <v>11</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>5</v>
       </c>
       <c r="J13" s="5">
@@ -2699,7 +2710,7 @@
         <f>AVERAGE(J13,K13,L13)</f>
         <v>10</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" s="7" t="s">
         <v>20</v>
       </c>
       <c r="P13" s="5">
@@ -2723,7 +2734,7 @@
       <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -2732,13 +2743,13 @@
       <c r="E14" s="5">
         <v>12</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="5">
@@ -2757,7 +2768,7 @@
         <f t="shared" si="0"/>
         <v>10.333333333333334</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="O14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="P14" s="5">
@@ -2781,7 +2792,7 @@
       <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -2790,7 +2801,7 @@
       <c r="E15" s="5">
         <v>13</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -2831,7 +2842,7 @@
         <v>13</v>
       </c>
       <c r="T15">
-        <f>AVERAGE(P15,Q15,R15)</f>
+        <f t="shared" ref="T15:T22" si="2">AVERAGE(P15,Q15,R15)</f>
         <v>9</v>
       </c>
     </row>
@@ -2854,7 +2865,7 @@
       <c r="G16" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="5">
@@ -2873,7 +2884,7 @@
         <f>AVERAGE(J16,K16,L16)</f>
         <v>14</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="O16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="P16" s="5">
@@ -2889,7 +2900,7 @@
         <v>14</v>
       </c>
       <c r="T16">
-        <f>AVERAGE(P16,Q16,R16)</f>
+        <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
     </row>
@@ -2912,7 +2923,7 @@
       <c r="G17" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J17" s="5">
@@ -2931,7 +2942,7 @@
         <f>AVERAGE(J17,K17,L17)</f>
         <v>15</v>
       </c>
-      <c r="O17" s="10" t="s">
+      <c r="O17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="P17" s="5">
@@ -2947,7 +2958,7 @@
         <v>15</v>
       </c>
       <c r="T17">
-        <f>AVERAGE(P17,Q17,R17)</f>
+        <f t="shared" si="2"/>
         <v>15.333333333333334</v>
       </c>
     </row>
@@ -2964,10 +2975,10 @@
       <c r="E18" s="5">
         <v>16</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="7" t="s">
         <v>101</v>
       </c>
       <c r="I18" s="5" t="s">
@@ -3005,7 +3016,7 @@
         <v>16</v>
       </c>
       <c r="T18">
-        <f>AVERAGE(P18,Q18,R18)</f>
+        <f t="shared" si="2"/>
         <v>16.333333333333332</v>
       </c>
     </row>
@@ -3063,7 +3074,7 @@
         <v>17</v>
       </c>
       <c r="T19">
-        <f>AVERAGE(P19,Q19,R19)</f>
+        <f t="shared" si="2"/>
         <v>15.666666666666666</v>
       </c>
     </row>
@@ -3121,7 +3132,7 @@
         <v>18</v>
       </c>
       <c r="T20">
-        <f>AVERAGE(P20,Q20,R20)</f>
+        <f t="shared" si="2"/>
         <v>16.666666666666668</v>
       </c>
     </row>
@@ -3179,7 +3190,7 @@
         <v>19</v>
       </c>
       <c r="T21">
-        <f>AVERAGE(P21,Q21,R21)</f>
+        <f t="shared" si="2"/>
         <v>19.666666666666668</v>
       </c>
     </row>
@@ -3237,7 +3248,7 @@
         <v>20</v>
       </c>
       <c r="T22">
-        <f>AVERAGE(P22,Q22,R22)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
     </row>
@@ -3304,10 +3315,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB5C47F-1FC5-024D-99B9-447C41AB77E5}">
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3321,16 +3332,17 @@
     <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" customWidth="1"/>
-    <col min="19" max="19" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.83203125" customWidth="1"/>
+    <col min="28" max="28" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="11" customWidth="1"/>
+    <col min="33" max="33" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17">
+    <row r="1" spans="1:33" ht="17">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -3357,29 +3369,59 @@
       <c r="L1" t="s">
         <v>114</v>
       </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="P1" t="s">
         <v>38</v>
       </c>
       <c r="Q1" t="s">
+        <v>118</v>
+      </c>
+      <c r="R1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="U1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" t="s">
         <v>110</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AA1" t="s">
         <v>111</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AB1" t="s">
         <v>40</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AC1" t="s">
         <v>112</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AD1" t="s">
         <v>115</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AE1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="17">
+    <row r="2" spans="1:33" ht="17">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -3407,39 +3449,68 @@
       <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="9">
         <v>25762310</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="O2" s="1">
+        <v>10</v>
+      </c>
+      <c r="P2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2">
+        <v>0.35129500000000002</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>18</v>
+      </c>
+      <c r="U2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q2">
+      <c r="Z2">
         <v>0.15768699999999999</v>
       </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <f>VLOOKUP(P2,A:C,3,0)</f>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <f>VLOOKUP(Y2,A:C,3,0)</f>
         <v>7</v>
       </c>
-      <c r="T2">
-        <f>VLOOKUP(P2,F:H,3,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <f>VLOOKUP(P2,K:M,3,0)</f>
+      <c r="AC2">
+        <f t="shared" ref="AC2:AC14" si="0">VLOOKUP(Y2,F:H,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <f t="shared" ref="AD2:AD23" si="1">VLOOKUP(Y2,K:M,3,0)</f>
         <v>3</v>
       </c>
-      <c r="V2" s="11">
-        <f>AVERAGE(R2,S2,T2,U2)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="17">
+      <c r="AE2">
+        <f>VLOOKUP(Y2,P:R,3,0)</f>
+        <v>2</v>
+      </c>
+      <c r="AF2">
+        <f>VLOOKUP(Y2,U:V,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="AG2" s="8">
+        <f>AVERAGE(AA2,AB2,AC2,AD2,AE2,AF2)</f>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="17">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3467,39 +3538,68 @@
       <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="9">
         <v>193453.6</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>16</v>
+      <c r="O3" s="1">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>7</v>
       </c>
       <c r="Q3">
-        <v>0.114978</v>
+        <v>0.339449</v>
       </c>
       <c r="R3">
         <v>2</v>
       </c>
-      <c r="S3">
-        <f t="shared" ref="S3:S5" si="0">VLOOKUP(P3,A:C,3,0)</f>
+      <c r="T3" s="1">
+        <v>2</v>
+      </c>
+      <c r="U3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3">
+        <v>0.114978</v>
+      </c>
+      <c r="AA3">
+        <v>2</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB5" si="2">VLOOKUP(Y3,A:C,3,0)</f>
         <v>4</v>
       </c>
-      <c r="T3">
-        <f>VLOOKUP(P3,F:H,3,0)</f>
+      <c r="AC3">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="U3">
-        <f>VLOOKUP(P3,K:M,3,0)</f>
+      <c r="AD3">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="V3" s="11">
-        <f t="shared" ref="V3:V14" si="1">AVERAGE(R3,S3,T3,U3)</f>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="17">
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE23" si="3">VLOOKUP(Y3,P:R,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" ref="AF3:AF22" si="4">VLOOKUP(Y3,U:V,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="AG3" s="8">
+        <f t="shared" ref="AG3:AG23" si="5">AVERAGE(AA3,AB3,AC3,AD3,AE3,AF3)</f>
+        <v>3.6666666666666665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="17">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -3527,39 +3627,68 @@
       <c r="K4" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="9">
         <v>86463.69</v>
       </c>
       <c r="M4">
         <v>3</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>24</v>
+      <c r="O4" s="1">
+        <v>4</v>
+      </c>
+      <c r="P4" t="s">
+        <v>9</v>
       </c>
       <c r="Q4">
-        <v>0.109038</v>
+        <v>0.31659799999999999</v>
       </c>
       <c r="R4">
         <v>3</v>
       </c>
-      <c r="S4">
+      <c r="T4" s="1">
+        <v>3</v>
+      </c>
+      <c r="U4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z4">
+        <v>0.109038</v>
+      </c>
+      <c r="AA4">
+        <v>3</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="AC4">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="T4">
-        <f>VLOOKUP(P4,F:H,3,0)</f>
         <v>3</v>
       </c>
-      <c r="U4">
-        <f>VLOOKUP(P4,K:M,3,0)</f>
+      <c r="AD4">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="V4" s="11">
-        <f t="shared" si="1"/>
-        <v>7.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="17">
+      <c r="AE4">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AG4" s="8">
+        <f t="shared" si="5"/>
+        <v>7.333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="17">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -3587,39 +3716,68 @@
       <c r="K5" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="9">
         <v>83312.570000000007</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>14</v>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>5</v>
       </c>
       <c r="Q5">
-        <v>8.6491999999999999E-2</v>
+        <v>0.25906200000000001</v>
       </c>
       <c r="R5">
         <v>4</v>
       </c>
-      <c r="S5">
+      <c r="T5" s="1">
+        <v>8</v>
+      </c>
+      <c r="U5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5">
+        <v>4</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z5">
+        <v>8.6491999999999999E-2</v>
+      </c>
+      <c r="AA5">
+        <v>4</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="AC5">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="T5">
-        <f>VLOOKUP(P5,F:H,3,0)</f>
         <v>4</v>
       </c>
-      <c r="U5">
-        <f>VLOOKUP(P5,K:M,3,0)</f>
+      <c r="AD5">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="V5" s="11">
-        <f t="shared" si="1"/>
+      <c r="AE5">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AG5" s="8">
+        <f t="shared" si="5"/>
         <v>8.5</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="17">
+    <row r="6" spans="1:33" ht="17">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -3647,39 +3805,68 @@
       <c r="K6" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="9">
         <v>65346.61</v>
       </c>
       <c r="M6">
         <v>5</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="O6" s="1">
+        <v>19</v>
+      </c>
+      <c r="P6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6">
+        <v>0.20352200000000001</v>
+      </c>
+      <c r="R6">
         <v>5</v>
       </c>
-      <c r="Q6">
+      <c r="T6" s="1">
+        <v>11</v>
+      </c>
+      <c r="U6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z6">
         <v>4.7012999999999999E-2</v>
       </c>
-      <c r="R6">
+      <c r="AA6">
         <v>7</v>
       </c>
-      <c r="S6">
-        <f>VLOOKUP(P6,A:C,3,0)</f>
+      <c r="AB6">
+        <f t="shared" ref="AB6:AB14" si="6">VLOOKUP(Y6,A:C,3,0)</f>
         <v>3</v>
       </c>
-      <c r="T6">
-        <f>VLOOKUP(P6,F:H,3,0)</f>
+      <c r="AC6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="U6">
-        <f>VLOOKUP(P6,K:M,3,0)</f>
+      <c r="AD6">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="V6" s="11">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="17">
+      <c r="AE6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="AG6" s="8">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="17">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -3707,39 +3894,68 @@
       <c r="K7" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="9">
         <v>43624.78</v>
       </c>
       <c r="M7">
         <v>6</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>0.12130199999999999</v>
+      </c>
+      <c r="R7">
+        <v>6</v>
+      </c>
+      <c r="T7" s="1">
+        <v>10</v>
+      </c>
+      <c r="U7" t="s">
+        <v>16</v>
+      </c>
+      <c r="V7">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q7">
+      <c r="Z7">
         <v>4.6096999999999999E-2</v>
       </c>
-      <c r="R7">
+      <c r="AA7">
         <v>8</v>
       </c>
-      <c r="S7">
-        <f>VLOOKUP(P7,A:C,3,0)</f>
+      <c r="AB7">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="T7">
-        <f>VLOOKUP(P7,F:H,3,0)</f>
+      <c r="AC7">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="U7">
-        <f>VLOOKUP(P7,K:M,3,0)</f>
+      <c r="AD7">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="V7" s="11">
-        <f t="shared" si="1"/>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="17">
+      <c r="AE7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AG7" s="8">
+        <f t="shared" si="5"/>
+        <v>7.666666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="17">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -3767,39 +3983,68 @@
       <c r="K8" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="9">
         <v>40073.31</v>
       </c>
       <c r="M8">
         <v>7</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="O8" s="1">
+        <v>13</v>
+      </c>
+      <c r="P8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8">
+        <v>7.5079999999999994E-2</v>
+      </c>
+      <c r="R8">
+        <v>7</v>
+      </c>
+      <c r="T8" s="1">
+        <v>19</v>
+      </c>
+      <c r="U8" t="s">
+        <v>25</v>
+      </c>
+      <c r="V8">
+        <v>7</v>
+      </c>
+      <c r="Y8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q8">
+      <c r="Z8">
         <v>4.0939999999999997E-2</v>
       </c>
-      <c r="R8">
+      <c r="AA8">
         <v>9</v>
       </c>
-      <c r="S8">
-        <f>VLOOKUP(P8,A:C,3,0)</f>
+      <c r="AB8">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="T8">
-        <f>VLOOKUP(P8,F:H,3,0)</f>
+      <c r="AC8">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="U8">
-        <f>VLOOKUP(P8,K:M,3,0)</f>
-        <v>1</v>
-      </c>
-      <c r="V8" s="11">
+      <c r="AD8">
         <f t="shared" si="1"/>
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="17">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="AG8" s="8">
+        <f t="shared" si="5"/>
+        <v>7.166666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="17">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -3827,39 +4072,68 @@
       <c r="K9" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="9">
         <v>35544.26</v>
       </c>
       <c r="M9">
         <v>8</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="O9" s="1">
+        <v>14</v>
+      </c>
+      <c r="P9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9">
+        <v>7.3971999999999996E-2</v>
+      </c>
+      <c r="R9">
+        <v>8</v>
+      </c>
+      <c r="T9" s="1">
+        <v>17</v>
+      </c>
+      <c r="U9" t="s">
+        <v>23</v>
+      </c>
+      <c r="V9">
+        <v>8</v>
+      </c>
+      <c r="Y9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q9">
+      <c r="Z9">
         <v>5.2641E-2</v>
       </c>
-      <c r="R9">
+      <c r="AA9">
         <v>6</v>
       </c>
-      <c r="S9">
-        <f>VLOOKUP(P9,A:C,3,0)</f>
+      <c r="AB9">
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="T9">
-        <f>VLOOKUP(P9,F:H,3,0)</f>
+      <c r="AC9">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="U9">
-        <f>VLOOKUP(P9,K:M,3,0)</f>
+      <c r="AD9">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="V9" s="11">
-        <f t="shared" si="1"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="17">
+      <c r="AE9">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="AG9" s="8">
+        <f t="shared" si="5"/>
+        <v>9.8333333333333339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="17">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -3887,39 +4161,68 @@
       <c r="K10" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="9">
         <v>34224.839999999997</v>
       </c>
       <c r="M10">
         <v>9</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="O10" s="1">
+        <v>12</v>
+      </c>
+      <c r="P10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10">
+        <v>3.0287999999999999E-2</v>
+      </c>
+      <c r="R10">
+        <v>9</v>
+      </c>
+      <c r="T10" s="1">
+        <v>7</v>
+      </c>
+      <c r="U10" t="s">
+        <v>13</v>
+      </c>
+      <c r="V10">
+        <v>9</v>
+      </c>
+      <c r="Y10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q10">
+      <c r="Z10">
         <v>3.8821000000000001E-2</v>
       </c>
-      <c r="R10">
+      <c r="AA10">
         <v>11</v>
       </c>
-      <c r="S10">
-        <f>VLOOKUP(P10,A:C,3,0)</f>
+      <c r="AB10">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="T10">
-        <f>VLOOKUP(P10,F:H,3,0)</f>
+      <c r="AC10">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="U10">
-        <f>VLOOKUP(P10,K:M,3,0)</f>
+      <c r="AD10">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="V10" s="11">
-        <f t="shared" si="1"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="17">
+      <c r="AE10">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="AG10" s="8">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="17">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -3947,39 +4250,64 @@
       <c r="K11" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="9">
         <v>19626.57</v>
       </c>
       <c r="M11">
         <v>10</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>8</v>
+      <c r="O11" s="1">
+        <v>20</v>
+      </c>
+      <c r="P11" t="s">
+        <v>26</v>
       </c>
       <c r="Q11">
-        <v>3.9614000000000003E-2</v>
+        <v>2.9517999999999999E-2</v>
       </c>
       <c r="R11">
         <v>10</v>
       </c>
-      <c r="S11">
-        <f>VLOOKUP(P11,A:C,3,0)</f>
+      <c r="T11" s="1">
+        <v>9</v>
+      </c>
+      <c r="U11" t="s">
         <v>15</v>
       </c>
-      <c r="T11">
-        <f>VLOOKUP(P11,F:H,3,0)</f>
+      <c r="V11">
+        <v>10</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z11">
+        <v>3.9614000000000003E-2</v>
+      </c>
+      <c r="AA11">
+        <v>10</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="U11">
-        <f>VLOOKUP(P11,K:M,3,0)</f>
+      <c r="AD11">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="V11" s="11">
-        <f t="shared" si="1"/>
-        <v>9.75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="17">
+      <c r="AF11">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="AG11" s="8">
+        <f>AVERAGE(AA11,AB11,AC11,AD11,AF11)</f>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="17">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -4007,39 +4335,68 @@
       <c r="K12" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="9">
         <v>16225.17</v>
       </c>
       <c r="M12">
         <v>11</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="O12" s="1">
+        <v>11</v>
+      </c>
+      <c r="P12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q12">
+        <v>8.2400000000000008E-3</v>
+      </c>
+      <c r="R12">
+        <v>11</v>
+      </c>
+      <c r="T12" s="1">
+        <v>12</v>
+      </c>
+      <c r="U12" t="s">
+        <v>18</v>
+      </c>
+      <c r="V12">
+        <v>11</v>
+      </c>
+      <c r="Y12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q12">
+      <c r="Z12">
         <v>2.5059000000000001E-2</v>
       </c>
-      <c r="R12">
+      <c r="AA12">
         <v>15</v>
       </c>
-      <c r="S12">
-        <f>VLOOKUP(P12,A:C,3,0)</f>
+      <c r="AB12">
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="T12">
-        <f>VLOOKUP(P12,F:H,3,0)</f>
+      <c r="AC12">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="U12">
-        <f>VLOOKUP(P12,K:M,3,0)</f>
+      <c r="AD12">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="V12" s="11">
-        <f t="shared" si="1"/>
-        <v>12.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="17">
+      <c r="AE12">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="AG12" s="8">
+        <f t="shared" si="5"/>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="17">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -4067,39 +4424,68 @@
       <c r="K13" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="9">
         <v>14378.31</v>
       </c>
       <c r="M13">
         <v>12</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="O13" s="1">
+        <v>7</v>
+      </c>
+      <c r="P13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13">
+        <v>-1.2090999999999999E-2</v>
+      </c>
+      <c r="R13">
+        <v>12</v>
+      </c>
+      <c r="T13" s="1">
+        <v>15</v>
+      </c>
+      <c r="U13" t="s">
+        <v>21</v>
+      </c>
+      <c r="V13">
+        <v>12</v>
+      </c>
+      <c r="Y13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q13">
+      <c r="Z13">
         <v>2.9742000000000001E-2</v>
       </c>
-      <c r="R13">
+      <c r="AA13">
         <v>13</v>
       </c>
-      <c r="S13">
-        <f>VLOOKUP(P13,A:C,3,0)</f>
+      <c r="AB13">
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="T13">
-        <f>VLOOKUP(P13,F:H,3,0)</f>
+      <c r="AC13">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="U13">
-        <f>VLOOKUP(P13,K:M,3,0)</f>
+      <c r="AD13">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="V13" s="11">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="17">
+      <c r="AE13">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="AG13" s="8">
+        <f t="shared" si="5"/>
+        <v>11.333333333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="17">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -4127,39 +4513,68 @@
       <c r="K14" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="9">
         <v>10548.61</v>
       </c>
       <c r="M14">
         <v>13</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="O14" s="1">
+        <v>8</v>
+      </c>
+      <c r="P14" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q14">
+        <v>-1.5325E-2</v>
+      </c>
+      <c r="R14">
+        <v>13</v>
+      </c>
+      <c r="T14" s="1">
         <v>20</v>
       </c>
-      <c r="Q14">
+      <c r="U14" t="s">
+        <v>26</v>
+      </c>
+      <c r="V14">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z14">
         <v>2.6262000000000001E-2</v>
       </c>
-      <c r="R14">
+      <c r="AA14">
         <v>14</v>
       </c>
-      <c r="S14">
-        <f>VLOOKUP(P14,A:C,3,0)</f>
+      <c r="AB14">
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="T14">
-        <f>VLOOKUP(P14,F:H,3,0)</f>
+      <c r="AC14">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="U14">
-        <f>VLOOKUP(P14,K:M,3,0)</f>
+      <c r="AD14">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="V14" s="11">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="17">
+      <c r="AE14">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="AF14">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="AG14" s="8">
+        <f t="shared" si="5"/>
+        <v>12.333333333333334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="17">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -4187,20 +4602,68 @@
       <c r="K15" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="9">
         <v>9225.3950000000004</v>
       </c>
       <c r="M15">
         <v>14</v>
       </c>
-      <c r="P15" s="1"/>
-      <c r="U15" t="e">
-        <f>VLOOKUP(P15,K:M,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V15" s="11"/>
-    </row>
-    <row r="16" spans="1:22" ht="17">
+      <c r="O15" s="1">
+        <v>18</v>
+      </c>
+      <c r="P15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15">
+        <v>-2.7560000000000001E-2</v>
+      </c>
+      <c r="R15">
+        <v>14</v>
+      </c>
+      <c r="T15" s="1">
+        <v>14</v>
+      </c>
+      <c r="U15" t="s">
+        <v>20</v>
+      </c>
+      <c r="V15">
+        <v>14</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z15">
+        <v>3.0306E-2</v>
+      </c>
+      <c r="AA15">
+        <v>12</v>
+      </c>
+      <c r="AB15">
+        <f>VLOOKUP(Y15,A:C,3,0)</f>
+        <v>19</v>
+      </c>
+      <c r="AC15">
+        <f>VLOOKUP(Y15,F:H,3,0)</f>
+        <v>12</v>
+      </c>
+      <c r="AD15">
+        <f>VLOOKUP(Y15,K:M,3,0)</f>
+        <v>18</v>
+      </c>
+      <c r="AE15">
+        <f>VLOOKUP(Y15,P:R,3,0)</f>
+        <v>16</v>
+      </c>
+      <c r="AF15">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AG15" s="8">
+        <f t="shared" si="5"/>
+        <v>14.166666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="17">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -4228,39 +4691,68 @@
       <c r="K16" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="9">
         <v>8493.6730000000007</v>
       </c>
       <c r="M16">
         <v>15</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>23</v>
+      <c r="O16" s="1">
+        <v>16</v>
+      </c>
+      <c r="P16" t="s">
+        <v>22</v>
       </c>
       <c r="Q16">
-        <v>3.0306E-2</v>
+        <v>-6.2001000000000001E-2</v>
       </c>
       <c r="R16">
-        <v>12</v>
-      </c>
-      <c r="S16">
-        <f>VLOOKUP(P16,A:C,3,0)</f>
+        <v>15</v>
+      </c>
+      <c r="T16" s="1">
+        <v>13</v>
+      </c>
+      <c r="U16" t="s">
         <v>19</v>
       </c>
-      <c r="T16">
-        <f>VLOOKUP(P16,F:H,3,0)</f>
-        <v>12</v>
-      </c>
-      <c r="U16">
-        <f>VLOOKUP(P16,K:M,3,0)</f>
-        <v>18</v>
-      </c>
-      <c r="V16" s="11">
-        <f t="shared" ref="V16:V22" si="2">AVERAGE(R16,S16,T16,U16)</f>
-        <v>15.25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="17">
+      <c r="V16">
+        <v>15</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z16">
+        <v>5.7054000000000001E-2</v>
+      </c>
+      <c r="AA16">
+        <v>5</v>
+      </c>
+      <c r="AB16">
+        <f>VLOOKUP(Y16,A:C,3,0)</f>
+        <v>22</v>
+      </c>
+      <c r="AC16">
+        <f>VLOOKUP(Y16,F:H,3,0)</f>
+        <v>19</v>
+      </c>
+      <c r="AD16">
+        <f>VLOOKUP(Y16,K:M,3,0)</f>
+        <v>21</v>
+      </c>
+      <c r="AE16">
+        <f>VLOOKUP(Y16,P:R,3,0)</f>
+        <v>11</v>
+      </c>
+      <c r="AF16">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AG16" s="8">
+        <f t="shared" si="5"/>
+        <v>13.833333333333334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" ht="17">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -4288,39 +4780,68 @@
       <c r="K17" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="9">
         <v>7019.9319999999998</v>
       </c>
       <c r="M17">
         <v>16</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="O17" s="1">
         <v>17</v>
       </c>
+      <c r="P17" t="s">
+        <v>23</v>
+      </c>
       <c r="Q17">
-        <v>5.7054000000000001E-2</v>
+        <v>-6.6786999999999999E-2</v>
       </c>
       <c r="R17">
-        <v>5</v>
-      </c>
-      <c r="S17">
-        <f>VLOOKUP(P17,A:C,3,0)</f>
+        <v>16</v>
+      </c>
+      <c r="T17" s="1">
+        <v>16</v>
+      </c>
+      <c r="U17" t="s">
         <v>22</v>
       </c>
-      <c r="T17">
-        <f>VLOOKUP(P17,F:H,3,0)</f>
+      <c r="V17">
+        <v>16</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z17">
+        <v>2.316E-2</v>
+      </c>
+      <c r="AA17">
+        <v>16</v>
+      </c>
+      <c r="AB17">
+        <f>VLOOKUP(Y17,A:C,3,0)</f>
+        <v>13</v>
+      </c>
+      <c r="AC17">
+        <f>VLOOKUP(Y17,F:H,3,0)</f>
+        <v>16</v>
+      </c>
+      <c r="AD17">
+        <f>VLOOKUP(Y17,K:M,3,0)</f>
         <v>19</v>
       </c>
-      <c r="U17">
-        <f>VLOOKUP(P17,K:M,3,0)</f>
-        <v>21</v>
-      </c>
-      <c r="V17" s="11">
-        <f t="shared" si="2"/>
-        <v>16.75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="17">
+      <c r="AE17">
+        <f>VLOOKUP(Y17,P:R,3,0)</f>
+        <v>10</v>
+      </c>
+      <c r="AF17">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="AG17" s="8">
+        <f t="shared" si="5"/>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" ht="17">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -4348,39 +4869,68 @@
       <c r="K18" t="s">
         <v>3</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="9">
         <v>6881.4449999999997</v>
       </c>
       <c r="M18">
         <v>17</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>26</v>
+      <c r="O18" s="1">
+        <v>15</v>
+      </c>
+      <c r="P18" t="s">
+        <v>21</v>
       </c>
       <c r="Q18">
-        <v>2.316E-2</v>
+        <v>-6.7368999999999998E-2</v>
       </c>
       <c r="R18">
+        <v>17</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0</v>
+      </c>
+      <c r="U18" t="s">
+        <v>3</v>
+      </c>
+      <c r="V18">
+        <v>17</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z18">
+        <v>2.1555000000000001E-2</v>
+      </c>
+      <c r="AA18">
+        <v>17</v>
+      </c>
+      <c r="AB18">
+        <f>VLOOKUP(Y18,A:C,3,0)</f>
+        <v>14</v>
+      </c>
+      <c r="AC18">
+        <f>VLOOKUP(Y18,F:H,3,0)</f>
+        <v>15</v>
+      </c>
+      <c r="AD18">
+        <f>VLOOKUP(Y18,K:M,3,0)</f>
         <v>16</v>
       </c>
-      <c r="S18">
-        <f>VLOOKUP(P18,A:C,3,0)</f>
-        <v>13</v>
-      </c>
-      <c r="T18">
-        <f>VLOOKUP(P18,F:H,3,0)</f>
-        <v>16</v>
-      </c>
-      <c r="U18">
-        <f>VLOOKUP(P18,K:M,3,0)</f>
-        <v>19</v>
-      </c>
-      <c r="V18" s="11">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="17">
+      <c r="AE18" t="e">
+        <f>VLOOKUP(Y18,P:R,3,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="AG18" s="8" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" ht="17">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -4408,39 +4958,56 @@
       <c r="K19" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="9">
         <v>6096.84</v>
       </c>
       <c r="M19">
         <v>18</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="T19" s="1">
+        <v>1</v>
+      </c>
+      <c r="U19" t="s">
+        <v>5</v>
+      </c>
+      <c r="V19">
+        <v>18</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z19">
+        <v>2.1267000000000001E-2</v>
+      </c>
+      <c r="AA19">
+        <v>18</v>
+      </c>
+      <c r="AB19">
+        <f>VLOOKUP(Y19,A:C,3,0)</f>
+        <v>12</v>
+      </c>
+      <c r="AC19">
+        <f>VLOOKUP(Y19,F:H,3,0)</f>
+        <v>18</v>
+      </c>
+      <c r="AD19">
+        <f>VLOOKUP(Y19,K:M,3,0)</f>
+        <v>20</v>
+      </c>
+      <c r="AE19">
+        <f>VLOOKUP(Y19,P:R,3,0)</f>
         <v>15</v>
       </c>
-      <c r="Q19">
-        <v>2.1555000000000001E-2</v>
-      </c>
-      <c r="R19">
-        <v>17</v>
-      </c>
-      <c r="S19">
-        <f>VLOOKUP(P19,A:C,3,0)</f>
-        <v>14</v>
-      </c>
-      <c r="T19">
-        <f>VLOOKUP(P19,F:H,3,0)</f>
-        <v>15</v>
-      </c>
-      <c r="U19">
-        <f>VLOOKUP(P19,K:M,3,0)</f>
+      <c r="AF19">
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="V19" s="11">
-        <f t="shared" si="2"/>
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="17">
+      <c r="AG19" s="8">
+        <f t="shared" si="5"/>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" ht="17">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -4468,39 +5035,56 @@
       <c r="K20" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="9">
         <v>5164.0619999999999</v>
       </c>
       <c r="M20">
         <v>19</v>
       </c>
-      <c r="P20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q20">
-        <v>2.1267000000000001E-2</v>
-      </c>
-      <c r="R20">
-        <v>18</v>
-      </c>
-      <c r="S20">
-        <f>VLOOKUP(P20,A:C,3,0)</f>
-        <v>12</v>
-      </c>
-      <c r="T20">
-        <f>VLOOKUP(P20,F:H,3,0)</f>
-        <v>18</v>
-      </c>
-      <c r="U20">
-        <f>VLOOKUP(P20,K:M,3,0)</f>
-        <v>20</v>
-      </c>
-      <c r="V20" s="11">
-        <f t="shared" si="2"/>
+      <c r="T20" s="1">
+        <v>6</v>
+      </c>
+      <c r="U20" t="s">
+        <v>11</v>
+      </c>
+      <c r="V20">
+        <v>19</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z20">
+        <v>1.1835E-2</v>
+      </c>
+      <c r="AA20">
+        <v>19</v>
+      </c>
+      <c r="AB20">
+        <f>VLOOKUP(Y20,A:C,3,0)</f>
+        <v>9</v>
+      </c>
+      <c r="AC20">
+        <f>VLOOKUP(Y20,F:H,3,0)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" ht="17">
+      <c r="AD20">
+        <f>VLOOKUP(Y20,K:M,3,0)</f>
+        <v>17</v>
+      </c>
+      <c r="AE20">
+        <f>VLOOKUP(Y20,P:R,3,0)</f>
+        <v>6</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="AG20" s="8">
+        <f t="shared" si="5"/>
+        <v>14.166666666666666</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" ht="17">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -4528,39 +5112,56 @@
       <c r="K21" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="9">
         <v>4379.09</v>
       </c>
       <c r="M21">
         <v>20</v>
       </c>
-      <c r="P21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q21">
-        <v>1.1835E-2</v>
-      </c>
-      <c r="R21">
+      <c r="T21" s="1">
+        <v>5</v>
+      </c>
+      <c r="U21" t="s">
+        <v>10</v>
+      </c>
+      <c r="V21">
+        <v>20</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z21">
+        <v>1.0298E-2</v>
+      </c>
+      <c r="AA21">
+        <v>20</v>
+      </c>
+      <c r="AB21">
+        <f>VLOOKUP(Y21,A:C,3,0)</f>
+        <v>20</v>
+      </c>
+      <c r="AC21">
+        <f>VLOOKUP(Y21,F:H,3,0)</f>
+        <v>20</v>
+      </c>
+      <c r="AD21">
+        <f>VLOOKUP(Y21,K:M,3,0)</f>
+        <v>4</v>
+      </c>
+      <c r="AE21" t="e">
+        <f>VLOOKUP(Y21,P:R,3,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AF21">
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="S21">
-        <f>VLOOKUP(P21,A:C,3,0)</f>
-        <v>9</v>
-      </c>
-      <c r="T21">
-        <f>VLOOKUP(P21,F:H,3,0)</f>
-        <v>17</v>
-      </c>
-      <c r="U21">
-        <f>VLOOKUP(P21,K:M,3,0)</f>
-        <v>17</v>
-      </c>
-      <c r="V21" s="11">
-        <f t="shared" si="2"/>
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="17">
+      <c r="AG21" s="8" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" ht="17">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -4576,39 +5177,52 @@
       <c r="K22" t="s">
         <v>17</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="9">
         <v>604.94569999999999</v>
       </c>
       <c r="M22">
         <v>21</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q22">
-        <v>1.0298E-2</v>
-      </c>
-      <c r="R22">
+      <c r="T22" s="1">
+        <v>4</v>
+      </c>
+      <c r="U22" t="s">
+        <v>9</v>
+      </c>
+      <c r="V22">
+        <v>21</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z22">
+        <v>1.0139E-2</v>
+      </c>
+      <c r="AA22">
+        <v>21</v>
+      </c>
+      <c r="AB22">
+        <f>VLOOKUP(Y22,A:C,3,0)</f>
+        <v>21</v>
+      </c>
+      <c r="AD22">
+        <f>VLOOKUP(Y22,K:M,3,0)</f>
+        <v>5</v>
+      </c>
+      <c r="AE22" t="e">
+        <f>VLOOKUP(Y22,P:R,3,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AF22">
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="S22">
-        <f>VLOOKUP(P22,A:C,3,0)</f>
-        <v>20</v>
-      </c>
-      <c r="T22">
-        <f>VLOOKUP(P22,F:H,3,0)</f>
-        <v>20</v>
-      </c>
-      <c r="U22">
-        <f>VLOOKUP(P22,K:M,3,0)</f>
-        <v>4</v>
-      </c>
-      <c r="V22" s="11">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" ht="17">
+      <c r="AG22" s="8" t="e">
+        <f t="shared" si="5"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" ht="17">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -4618,34 +5232,17 @@
       <c r="C23">
         <v>22</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q23">
-        <v>1.0139E-2</v>
-      </c>
-      <c r="R23">
-        <v>21</v>
-      </c>
-      <c r="S23">
-        <f>VLOOKUP(P23,A:C,3,0)</f>
-        <v>21</v>
-      </c>
-      <c r="U23">
-        <f>VLOOKUP(P23,K:M,3,0)</f>
-        <v>5</v>
-      </c>
-      <c r="V23" s="11">
-        <f>AVERAGE(R23,S23,T23,U23)</f>
-        <v>15.666666666666666</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22">
+      <c r="AG23" s="8" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33">
       <c r="A29" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="17">
+    <row r="30" spans="1:33" ht="17">
       <c r="A30" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
Changes to Feature selection & clustering
</commit_message>
<xml_diff>
--- a/documentation/week2/Feature_selection.xlsx
+++ b/documentation/week2/Feature_selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharakumarrathinar/Documents/MS_Heriot_Watt/Course_work/F21DL/code/documentation/week2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A2A5C9-A8F5-E543-9406-479339A3E85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73C0FDE-CF47-674E-9DA3-F33CF499E310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20960" activeTab="3" xr2:uid="{416BFC02-E214-EC46-9E71-DF9EF0F7F4BC}"/>
+    <workbookView xWindow="7600" yWindow="500" windowWidth="36000" windowHeight="20960" activeTab="3" xr2:uid="{416BFC02-E214-EC46-9E71-DF9EF0F7F4BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -3318,7 +3318,7 @@
   <dimension ref="A1:AG30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7"/>
+      <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Folder Structure change & Final Document push
</commit_message>
<xml_diff>
--- a/documentation/week2/Feature_selection.xlsx
+++ b/documentation/week2/Feature_selection.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hariharakumarrathinar/Documents/MS_Heriot_Watt/Course_work/F21DL/code/documentation/week2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73C0FDE-CF47-674E-9DA3-F33CF499E310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75656C1F-F462-644F-9959-DDD1D03F55F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="500" windowWidth="36000" windowHeight="20960" activeTab="3" xr2:uid="{416BFC02-E214-EC46-9E71-DF9EF0F7F4BC}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20940" activeTab="3" xr2:uid="{416BFC02-E214-EC46-9E71-DF9EF0F7F4BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +471,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,7 +518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -529,6 +535,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -550,7 +559,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -558,34 +567,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -3317,29 +3326,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB5C47F-1FC5-024D-99B9-447C41AB77E5}">
   <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.83203125" customWidth="1"/>
-    <col min="28" max="28" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="11" customWidth="1"/>
-    <col min="33" max="33" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="17">
@@ -3393,31 +3412,31 @@
       <c r="V1" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="14" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3476,36 +3495,36 @@
       <c r="V2">
         <v>1</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="5">
         <v>0.15768699999999999</v>
       </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
+      <c r="AA2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="5">
         <f>VLOOKUP(Y2,A:C,3,0)</f>
         <v>7</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="5">
         <f t="shared" ref="AC2:AC14" si="0">VLOOKUP(Y2,F:H,3,0)</f>
         <v>1</v>
       </c>
-      <c r="AD2">
-        <f t="shared" ref="AD2:AD23" si="1">VLOOKUP(Y2,K:M,3,0)</f>
+      <c r="AD2" s="5">
+        <f t="shared" ref="AD2:AD14" si="1">VLOOKUP(Y2,K:M,3,0)</f>
         <v>3</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="5">
         <f>VLOOKUP(Y2,P:R,3,0)</f>
         <v>2</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="5">
         <f>VLOOKUP(Y2,U:V,2,0)</f>
         <v>2</v>
       </c>
-      <c r="AG2" s="8">
+      <c r="AG2" s="13">
         <f>AVERAGE(AA2,AB2,AC2,AD2,AE2,AF2)</f>
         <v>2.6666666666666665</v>
       </c>
@@ -3565,36 +3584,36 @@
       <c r="V3">
         <v>2</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Y3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="5">
         <v>0.114978</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="5">
         <v>2</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="5">
         <f t="shared" ref="AB3:AB5" si="2">VLOOKUP(Y3,A:C,3,0)</f>
         <v>4</v>
       </c>
-      <c r="AC3">
+      <c r="AC3" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AD3">
+      <c r="AD3" s="5">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="AE3">
-        <f t="shared" ref="AE3:AE23" si="3">VLOOKUP(Y3,P:R,3,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AF3">
+      <c r="AE3" s="5">
+        <f t="shared" ref="AE3:AE14" si="3">VLOOKUP(Y3,P:R,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF3" s="5">
         <f t="shared" ref="AF3:AF22" si="4">VLOOKUP(Y3,U:V,2,0)</f>
         <v>6</v>
       </c>
-      <c r="AG3" s="8">
+      <c r="AG3" s="13">
         <f t="shared" ref="AG3:AG23" si="5">AVERAGE(AA3,AB3,AC3,AD3,AE3,AF3)</f>
         <v>3.6666666666666665</v>
       </c>
@@ -3654,36 +3673,36 @@
       <c r="V4">
         <v>3</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Y4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="5">
         <v>0.109038</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="5">
         <v>3</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="5">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="5">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="AG4" s="8">
+      <c r="AG4" s="13">
         <f t="shared" si="5"/>
         <v>7.333333333333333</v>
       </c>
@@ -3743,36 +3762,36 @@
       <c r="V5">
         <v>4</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Y5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="5">
         <v>8.6491999999999999E-2</v>
       </c>
-      <c r="AA5">
+      <c r="AA5" s="5">
         <v>4</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="5">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="AC5">
+      <c r="AC5" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="AD5">
+      <c r="AD5" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="5">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="AF5">
+      <c r="AF5" s="5">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="AG5" s="8">
+      <c r="AG5" s="13">
         <f t="shared" si="5"/>
         <v>8.5</v>
       </c>
@@ -3832,36 +3851,36 @@
       <c r="V6">
         <v>5</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Y6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="5">
         <v>4.7012999999999999E-2</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="5">
         <v>7</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="5">
         <f t="shared" ref="AB6:AB14" si="6">VLOOKUP(Y6,A:C,3,0)</f>
         <v>3</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="AD6">
+      <c r="AD6" s="5">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="5">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="AF6">
+      <c r="AF6" s="5">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="AG6" s="8">
+      <c r="AG6" s="13">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
@@ -3921,36 +3940,36 @@
       <c r="V7">
         <v>6</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Y7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="5">
         <v>4.6096999999999999E-2</v>
       </c>
-      <c r="AA7">
+      <c r="AA7" s="5">
         <v>8</v>
       </c>
-      <c r="AB7">
+      <c r="AB7" s="5">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="AC7">
+      <c r="AC7" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AD7">
+      <c r="AD7" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="AE7">
+      <c r="AE7" s="5">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="AF7">
+      <c r="AF7" s="5">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="AG7" s="8">
+      <c r="AG7" s="13">
         <f t="shared" si="5"/>
         <v>7.666666666666667</v>
       </c>
@@ -4010,36 +4029,36 @@
       <c r="V8">
         <v>7</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="Y8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="5">
         <v>4.0939999999999997E-2</v>
       </c>
-      <c r="AA8">
+      <c r="AA8" s="5">
         <v>9</v>
       </c>
-      <c r="AB8">
+      <c r="AB8" s="5">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="AC8">
+      <c r="AC8" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="AD8">
+      <c r="AD8" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AE8">
+      <c r="AE8" s="5">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="AF8">
+      <c r="AF8" s="5">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="AG8" s="8">
+      <c r="AG8" s="13">
         <f t="shared" si="5"/>
         <v>7.166666666666667</v>
       </c>
@@ -4099,36 +4118,36 @@
       <c r="V9">
         <v>8</v>
       </c>
-      <c r="Y9" s="1" t="s">
+      <c r="Y9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="5">
         <v>5.2641E-2</v>
       </c>
-      <c r="AA9">
+      <c r="AA9" s="5">
         <v>6</v>
       </c>
-      <c r="AB9">
+      <c r="AB9" s="5">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="AC9">
+      <c r="AC9" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="AD9">
+      <c r="AD9" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="AE9">
+      <c r="AE9" s="5">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="AF9">
+      <c r="AF9" s="5">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="AG9" s="8">
+      <c r="AG9" s="13">
         <f t="shared" si="5"/>
         <v>9.8333333333333339</v>
       </c>
@@ -4188,36 +4207,36 @@
       <c r="V10">
         <v>9</v>
       </c>
-      <c r="Y10" s="1" t="s">
+      <c r="Y10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="5">
         <v>3.8821000000000001E-2</v>
       </c>
-      <c r="AA10">
+      <c r="AA10" s="5">
         <v>11</v>
       </c>
-      <c r="AB10">
+      <c r="AB10" s="5">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="AC10">
+      <c r="AC10" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="AD10">
+      <c r="AD10" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="AE10">
+      <c r="AE10" s="5">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="AF10">
+      <c r="AF10" s="5">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="AG10" s="8">
+      <c r="AG10" s="13">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
@@ -4277,34 +4296,37 @@
       <c r="V11">
         <v>10</v>
       </c>
-      <c r="Y11" s="1" t="s">
+      <c r="Y11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="5">
         <v>3.9614000000000003E-2</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="5">
         <v>10</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="5">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="AD11">
+      <c r="AD11" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="AF11">
+      <c r="AE11" s="5">
+        <v>22</v>
+      </c>
+      <c r="AF11" s="5">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="AG11" s="8">
-        <f>AVERAGE(AA11,AB11,AC11,AD11,AF11)</f>
-        <v>8.4</v>
+      <c r="AG11" s="13">
+        <f t="shared" si="5"/>
+        <v>10.666666666666666</v>
       </c>
     </row>
     <row r="12" spans="1:33" ht="17">
@@ -4362,36 +4384,36 @@
       <c r="V12">
         <v>11</v>
       </c>
-      <c r="Y12" s="1" t="s">
+      <c r="Y12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="5">
         <v>2.5059000000000001E-2</v>
       </c>
-      <c r="AA12">
+      <c r="AA12" s="5">
         <v>15</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="5">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="AC12">
+      <c r="AC12" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="AD12">
+      <c r="AD12" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="AE12">
+      <c r="AE12" s="5">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="AF12">
+      <c r="AF12" s="5">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="AG12" s="8">
+      <c r="AG12" s="13">
         <f t="shared" si="5"/>
         <v>13.333333333333334</v>
       </c>
@@ -4451,36 +4473,36 @@
       <c r="V13">
         <v>12</v>
       </c>
-      <c r="Y13" s="1" t="s">
+      <c r="Y13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="5">
         <v>2.9742000000000001E-2</v>
       </c>
-      <c r="AA13">
+      <c r="AA13" s="5">
         <v>13</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="5">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="AC13">
+      <c r="AC13" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AD13">
+      <c r="AD13" s="5">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="5">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="AF13">
+      <c r="AF13" s="5">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="AG13" s="8">
+      <c r="AG13" s="13">
         <f t="shared" si="5"/>
         <v>11.333333333333334</v>
       </c>
@@ -4540,36 +4562,36 @@
       <c r="V14">
         <v>13</v>
       </c>
-      <c r="Y14" s="1" t="s">
+      <c r="Y14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="Z14">
+      <c r="Z14" s="5">
         <v>2.6262000000000001E-2</v>
       </c>
-      <c r="AA14">
+      <c r="AA14" s="5">
         <v>14</v>
       </c>
-      <c r="AB14">
+      <c r="AB14" s="5">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="AC14">
+      <c r="AC14" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="AD14">
+      <c r="AD14" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="AE14">
+      <c r="AE14" s="5">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="AF14">
+      <c r="AF14" s="5">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="AG14" s="8">
+      <c r="AG14" s="13">
         <f t="shared" si="5"/>
         <v>12.333333333333334</v>
       </c>
@@ -4629,36 +4651,36 @@
       <c r="V15">
         <v>14</v>
       </c>
-      <c r="Y15" s="1" t="s">
+      <c r="Y15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="5">
         <v>3.0306E-2</v>
       </c>
-      <c r="AA15">
+      <c r="AA15" s="5">
         <v>12</v>
       </c>
-      <c r="AB15">
-        <f>VLOOKUP(Y15,A:C,3,0)</f>
+      <c r="AB15" s="5">
+        <f t="shared" ref="AB15:AB22" si="7">VLOOKUP(Y15,A:C,3,0)</f>
         <v>19</v>
       </c>
-      <c r="AC15">
-        <f>VLOOKUP(Y15,F:H,3,0)</f>
+      <c r="AC15" s="5">
+        <f t="shared" ref="AC15:AC21" si="8">VLOOKUP(Y15,F:H,3,0)</f>
         <v>12</v>
       </c>
-      <c r="AD15">
-        <f>VLOOKUP(Y15,K:M,3,0)</f>
+      <c r="AD15" s="5">
+        <f t="shared" ref="AD15:AD22" si="9">VLOOKUP(Y15,K:M,3,0)</f>
         <v>18</v>
       </c>
-      <c r="AE15">
-        <f>VLOOKUP(Y15,P:R,3,0)</f>
+      <c r="AE15" s="5">
+        <f t="shared" ref="AE15:AE22" si="10">VLOOKUP(Y15,P:R,3,0)</f>
         <v>16</v>
       </c>
-      <c r="AF15">
+      <c r="AF15" s="5">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="AG15" s="8">
+      <c r="AG15" s="13">
         <f t="shared" si="5"/>
         <v>14.166666666666666</v>
       </c>
@@ -4718,36 +4740,36 @@
       <c r="V16">
         <v>15</v>
       </c>
-      <c r="Y16" s="1" t="s">
+      <c r="Y16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Z16">
+      <c r="Z16" s="5">
         <v>5.7054000000000001E-2</v>
       </c>
-      <c r="AA16">
+      <c r="AA16" s="5">
         <v>5</v>
       </c>
-      <c r="AB16">
-        <f>VLOOKUP(Y16,A:C,3,0)</f>
+      <c r="AB16" s="5">
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
-      <c r="AC16">
-        <f>VLOOKUP(Y16,F:H,3,0)</f>
+      <c r="AC16" s="5">
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
-      <c r="AD16">
-        <f>VLOOKUP(Y16,K:M,3,0)</f>
+      <c r="AD16" s="5">
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
-      <c r="AE16">
-        <f>VLOOKUP(Y16,P:R,3,0)</f>
+      <c r="AE16" s="5">
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="AF16">
+      <c r="AF16" s="5">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="AG16" s="8">
+      <c r="AG16" s="13">
         <f t="shared" si="5"/>
         <v>13.833333333333334</v>
       </c>
@@ -4807,36 +4829,36 @@
       <c r="V17">
         <v>16</v>
       </c>
-      <c r="Y17" s="1" t="s">
+      <c r="Y17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="5">
         <v>2.316E-2</v>
       </c>
-      <c r="AA17">
+      <c r="AA17" s="5">
         <v>16</v>
       </c>
-      <c r="AB17">
-        <f>VLOOKUP(Y17,A:C,3,0)</f>
+      <c r="AB17" s="5">
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
-      <c r="AC17">
-        <f>VLOOKUP(Y17,F:H,3,0)</f>
+      <c r="AC17" s="5">
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="AD17">
-        <f>VLOOKUP(Y17,K:M,3,0)</f>
+      <c r="AD17" s="5">
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
-      <c r="AE17">
-        <f>VLOOKUP(Y17,P:R,3,0)</f>
+      <c r="AE17" s="5">
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="AF17">
+      <c r="AF17" s="5">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="AG17" s="8">
+      <c r="AG17" s="13">
         <f t="shared" si="5"/>
         <v>14.5</v>
       </c>
@@ -4896,38 +4918,37 @@
       <c r="V18">
         <v>17</v>
       </c>
-      <c r="Y18" s="1" t="s">
+      <c r="Y18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="5">
         <v>2.1555000000000001E-2</v>
       </c>
-      <c r="AA18">
+      <c r="AA18" s="5">
         <v>17</v>
       </c>
-      <c r="AB18">
-        <f>VLOOKUP(Y18,A:C,3,0)</f>
+      <c r="AB18" s="5">
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="AC18">
-        <f>VLOOKUP(Y18,F:H,3,0)</f>
+      <c r="AC18" s="5">
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
-      <c r="AD18">
-        <f>VLOOKUP(Y18,K:M,3,0)</f>
+      <c r="AD18" s="5">
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="AE18" t="e">
-        <f>VLOOKUP(Y18,P:R,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AF18">
+      <c r="AE18" s="5">
+        <v>22</v>
+      </c>
+      <c r="AF18" s="5">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="AG18" s="8" t="e">
+      <c r="AG18" s="13">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>15.666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="17">
@@ -4973,36 +4994,36 @@
       <c r="V19">
         <v>18</v>
       </c>
-      <c r="Y19" s="1" t="s">
+      <c r="Y19" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" s="5">
         <v>2.1267000000000001E-2</v>
       </c>
-      <c r="AA19">
+      <c r="AA19" s="5">
         <v>18</v>
       </c>
-      <c r="AB19">
-        <f>VLOOKUP(Y19,A:C,3,0)</f>
+      <c r="AB19" s="5">
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="AC19">
-        <f>VLOOKUP(Y19,F:H,3,0)</f>
+      <c r="AC19" s="5">
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="AD19">
-        <f>VLOOKUP(Y19,K:M,3,0)</f>
+      <c r="AD19" s="5">
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
-      <c r="AE19">
-        <f>VLOOKUP(Y19,P:R,3,0)</f>
+      <c r="AE19" s="5">
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
-      <c r="AF19">
+      <c r="AF19" s="5">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="AG19" s="8">
+      <c r="AG19" s="13">
         <f t="shared" si="5"/>
         <v>16.5</v>
       </c>
@@ -5050,36 +5071,36 @@
       <c r="V20">
         <v>19</v>
       </c>
-      <c r="Y20" s="1" t="s">
+      <c r="Y20" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="5">
         <v>1.1835E-2</v>
       </c>
-      <c r="AA20">
+      <c r="AA20" s="5">
         <v>19</v>
       </c>
-      <c r="AB20">
-        <f>VLOOKUP(Y20,A:C,3,0)</f>
+      <c r="AB20" s="5">
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="AC20">
-        <f>VLOOKUP(Y20,F:H,3,0)</f>
+      <c r="AC20" s="5">
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
-      <c r="AD20">
-        <f>VLOOKUP(Y20,K:M,3,0)</f>
+      <c r="AD20" s="5">
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
-      <c r="AE20">
-        <f>VLOOKUP(Y20,P:R,3,0)</f>
+      <c r="AE20" s="5">
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
-      <c r="AF20">
+      <c r="AF20" s="5">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="AG20" s="8">
+      <c r="AG20" s="13">
         <f t="shared" si="5"/>
         <v>14.166666666666666</v>
       </c>
@@ -5127,38 +5148,37 @@
       <c r="V21">
         <v>20</v>
       </c>
-      <c r="Y21" s="1" t="s">
+      <c r="Y21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="5">
         <v>1.0298E-2</v>
       </c>
-      <c r="AA21">
+      <c r="AA21" s="5">
         <v>20</v>
       </c>
-      <c r="AB21">
-        <f>VLOOKUP(Y21,A:C,3,0)</f>
+      <c r="AB21" s="5">
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="AC21">
-        <f>VLOOKUP(Y21,F:H,3,0)</f>
+      <c r="AC21" s="5">
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="AD21">
-        <f>VLOOKUP(Y21,K:M,3,0)</f>
+      <c r="AD21" s="5">
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="AE21" t="e">
-        <f>VLOOKUP(Y21,P:R,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AF21">
+      <c r="AE21" s="5">
+        <v>22</v>
+      </c>
+      <c r="AF21" s="5">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="AG21" s="8" t="e">
+      <c r="AG21" s="13">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="22" spans="1:33" ht="17">
@@ -5192,34 +5212,34 @@
       <c r="V22">
         <v>21</v>
       </c>
-      <c r="Y22" s="1" t="s">
+      <c r="Y22" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Z22">
+      <c r="Z22" s="5">
         <v>1.0139E-2</v>
       </c>
-      <c r="AA22">
+      <c r="AA22" s="5">
         <v>21</v>
       </c>
-      <c r="AB22">
-        <f>VLOOKUP(Y22,A:C,3,0)</f>
+      <c r="AB22" s="5">
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
-      <c r="AD22">
-        <f>VLOOKUP(Y22,K:M,3,0)</f>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5">
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="AE22" t="e">
-        <f>VLOOKUP(Y22,P:R,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AF22">
+      <c r="AE22" s="5">
+        <v>22</v>
+      </c>
+      <c r="AF22" s="5">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="AG22" s="8" t="e">
+      <c r="AG22" s="13">
         <f t="shared" si="5"/>
-        <v>#N/A</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="23" spans="1:33" ht="17">
@@ -5232,10 +5252,7 @@
       <c r="C23">
         <v>22</v>
       </c>
-      <c r="AG23" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="AG23" s="8"/>
     </row>
     <row r="29" spans="1:33">
       <c r="A29" t="s">

</xml_diff>